<commit_message>
1)customer and dealer UI done. 2)able to fetch data based on date and customer type. stock and profit needed work. 2 hours work remaining
</commit_message>
<xml_diff>
--- a/downloads/temp.xlsx
+++ b/downloads/temp.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="46">
   <si>
     <t>Id</t>
   </si>
@@ -125,6 +125,30 @@
   </si>
   <si>
     <t>790</t>
+  </si>
+  <si>
+    <t>shgda</t>
+  </si>
+  <si>
+    <t>jlwdkas</t>
+  </si>
+  <si>
+    <t>kjl</t>
+  </si>
+  <si>
+    <t>2018-09-15</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>131</t>
   </si>
 </sst>
 </file>
@@ -508,7 +532,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O15"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
@@ -816,6 +840,334 @@
         <v>2.9600000000000364</v>
       </c>
     </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12">
+        <v>34</v>
+      </c>
+      <c r="K12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12">
+        <v>164.9</v>
+      </c>
+      <c r="N12" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12">
+        <v>33.900000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13">
+        <v>164.9</v>
+      </c>
+      <c r="N13" t="s">
+        <v>45</v>
+      </c>
+      <c r="O13">
+        <v>33.900000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" t="s">
+        <v>44</v>
+      </c>
+      <c r="M14">
+        <v>164.9</v>
+      </c>
+      <c r="N14" t="s">
+        <v>45</v>
+      </c>
+      <c r="O14">
+        <v>33.900000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
excel name change remaining
</commit_message>
<xml_diff>
--- a/downloads/temp.xlsx
+++ b/downloads/temp.xlsx
@@ -453,19 +453,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>7860</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>11130</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>13234</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>-32224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all done and tested
</commit_message>
<xml_diff>
--- a/downloads/temp.xlsx
+++ b/downloads/temp.xlsx
@@ -11,27 +11,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Dealer - 09 - 2018</t>
+  </si>
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Stock</t>
+    <t>Date</t>
   </si>
   <si>
     <t>Dealer</t>
   </si>
   <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>miscellaneous</t>
-  </si>
-  <si>
-    <t>Amount Pending</t>
-  </si>
-  <si>
-    <t>Profit</t>
+    <t>Cylinder Size</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Net Amount</t>
+  </si>
+  <si>
+    <t>Amount Paid</t>
+  </si>
+  <si>
+    <t>Amount Due</t>
+  </si>
+  <si>
+    <t>2018-09-02</t>
+  </si>
+  <si>
+    <t>abhishek chu</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>786</t>
+  </si>
+  <si>
+    <t>7869</t>
   </si>
 </sst>
 </file>
@@ -415,60 +442,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="7" width="23" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="9" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="3:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>7860</v>
-      </c>
-      <c r="D2">
-        <v>11130</v>
-      </c>
-      <c r="E2">
-        <v>13234</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>-32224</v>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>78600</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>70731</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
remove redundant mandatory field, changed address
</commit_message>
<xml_diff>
--- a/downloads/temp.xlsx
+++ b/downloads/temp.xlsx
@@ -11,33 +11,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Miscellaneous - 11 - 2018</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Profit - whole - 2019</t>
   </si>
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Net Amount</t>
-  </si>
-  <si>
-    <t>2018-11-01</t>
-  </si>
-  <si>
-    <t>petrol</t>
-  </si>
-  <si>
-    <t>2018-11-23</t>
-  </si>
-  <si>
-    <t>Petrol</t>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Dealer</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Amount Pending</t>
+  </si>
+  <si>
+    <t>Profit</t>
   </si>
 </sst>
 </file>
@@ -421,13 +418,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="2" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -442,7 +437,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -455,33 +450,37 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>